<commit_message>
datasets before last matchday
</commit_message>
<xml_diff>
--- a/data/out/wiki/men/fifa/wc/goals_wc_fifa_men.xlsx
+++ b/data/out/wiki/men/fifa/wc/goals_wc_fifa_men.xlsx
@@ -633,7 +633,7 @@
       <c r="I2" t="inlineStr"/>
       <c r="J2" t="inlineStr">
         <is>
-          <t>['France', 'Hungary', 'Soviet Union']</t>
+          <t>['Hungary', 'France', 'Soviet Union']</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
@@ -729,7 +729,7 @@
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>['France', 'Hungary', 'Soviet Union']</t>
+          <t>['Hungary', 'France', 'Soviet Union']</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
@@ -857,7 +857,7 @@
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>['France', 'Hungary', 'Soviet Union']</t>
+          <t>['Hungary', 'France', 'Soviet Union']</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
@@ -985,7 +985,7 @@
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>['France', 'Hungary', 'Soviet Union']</t>
+          <t>['Hungary', 'France', 'Soviet Union']</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
@@ -1113,7 +1113,7 @@
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>['France', 'Hungary', 'Soviet Union']</t>
+          <t>['Hungary', 'France', 'Soviet Union']</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
@@ -1241,7 +1241,7 @@
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>['France', 'Hungary', 'Soviet Union']</t>
+          <t>['Hungary', 'France', 'Soviet Union']</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
@@ -1355,7 +1355,7 @@
       <c r="I8" t="inlineStr"/>
       <c r="J8" t="inlineStr">
         <is>
-          <t>['Bulgaria', 'Italy', 'Argentina']</t>
+          <t>['Italy', 'Argentina', 'Bulgaria']</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
@@ -1451,7 +1451,7 @@
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>['Bulgaria', 'Italy', 'Argentina']</t>
+          <t>['Italy', 'Argentina', 'Bulgaria']</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
@@ -1579,7 +1579,7 @@
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>['Bulgaria', 'Italy', 'Argentina']</t>
+          <t>['Italy', 'Argentina', 'Bulgaria']</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
@@ -1707,7 +1707,7 @@
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>['Bulgaria', 'Italy', 'Argentina']</t>
+          <t>['Italy', 'Argentina', 'Bulgaria']</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
@@ -1835,7 +1835,7 @@
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>['Bulgaria', 'Italy', 'Argentina']</t>
+          <t>['Italy', 'Argentina', 'Bulgaria']</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
@@ -1963,7 +1963,7 @@
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>['Bulgaria', 'Italy', 'Argentina']</t>
+          <t>['Italy', 'Argentina', 'Bulgaria']</t>
         </is>
       </c>
       <c r="K13" t="inlineStr">
@@ -2091,7 +2091,7 @@
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>['Bulgaria', 'Italy', 'Argentina']</t>
+          <t>['Italy', 'Argentina', 'Bulgaria']</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
@@ -2219,7 +2219,7 @@
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>['Bulgaria', 'Italy', 'Argentina']</t>
+          <t>['Italy', 'Argentina', 'Bulgaria']</t>
         </is>
       </c>
       <c r="K15" t="inlineStr">
@@ -2333,7 +2333,7 @@
       <c r="I16" t="inlineStr"/>
       <c r="J16" t="inlineStr">
         <is>
-          <t>['Paraguay', 'Belgium', 'Mexico']</t>
+          <t>['Paraguay', 'Mexico', 'Belgium']</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
@@ -2429,7 +2429,7 @@
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>['Belgium', 'Mexico', 'Paraguay']</t>
+          <t>['Paraguay', 'Mexico', 'Belgium']</t>
         </is>
       </c>
       <c r="K17" t="inlineStr">
@@ -2557,7 +2557,7 @@
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>['Paraguay', 'Belgium', 'Mexico']</t>
+          <t>['Paraguay', 'Mexico', 'Belgium']</t>
         </is>
       </c>
       <c r="K18" t="inlineStr">
@@ -2685,7 +2685,7 @@
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>['Paraguay', 'Belgium', 'Mexico']</t>
+          <t>['Paraguay', 'Mexico', 'Belgium']</t>
         </is>
       </c>
       <c r="K19" t="inlineStr">
@@ -2813,7 +2813,7 @@
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>['Belgium', 'Mexico', 'Paraguay']</t>
+          <t>['Paraguay', 'Mexico', 'Belgium']</t>
         </is>
       </c>
       <c r="K20" t="inlineStr">
@@ -2941,7 +2941,7 @@
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>['Paraguay', 'Belgium', 'Mexico']</t>
+          <t>['Paraguay', 'Mexico', 'Belgium']</t>
         </is>
       </c>
       <c r="K21" t="inlineStr">
@@ -3055,7 +3055,7 @@
       <c r="I22" t="inlineStr"/>
       <c r="J22" t="inlineStr">
         <is>
-          <t>['Poland', 'Portugal', 'Morocco']</t>
+          <t>['Morocco', 'Poland', 'Portugal']</t>
         </is>
       </c>
       <c r="K22" t="inlineStr">
@@ -3279,7 +3279,7 @@
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>['England', 'Portugal', 'Morocco']</t>
+          <t>['Morocco', 'Portugal', 'England']</t>
         </is>
       </c>
       <c r="K24" t="inlineStr">
@@ -3407,7 +3407,7 @@
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>['England', 'Poland', 'Morocco']</t>
+          <t>['Poland', 'Morocco', 'England']</t>
         </is>
       </c>
       <c r="K25" t="inlineStr">
@@ -3535,7 +3535,7 @@
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>['England', 'Poland', 'Morocco']</t>
+          <t>['Poland', 'Morocco', 'England']</t>
         </is>
       </c>
       <c r="K26" t="inlineStr">
@@ -3663,7 +3663,7 @@
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>['England', 'Poland', 'Morocco']</t>
+          <t>['Poland', 'Morocco', 'England']</t>
         </is>
       </c>
       <c r="K27" t="inlineStr">
@@ -3791,7 +3791,7 @@
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>['England', 'Poland', 'Morocco']</t>
+          <t>['Poland', 'Morocco', 'England']</t>
         </is>
       </c>
       <c r="K28" t="inlineStr">
@@ -3919,7 +3919,7 @@
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>['England', 'Poland', 'Morocco']</t>
+          <t>['Poland', 'Morocco', 'England']</t>
         </is>
       </c>
       <c r="K29" t="inlineStr">
@@ -4033,7 +4033,7 @@
       <c r="I30" t="inlineStr"/>
       <c r="J30" t="inlineStr">
         <is>
-          <t>['Spain', 'Northern Ireland', 'Brazil']</t>
+          <t>['Brazil', 'Spain', 'Northern Ireland']</t>
         </is>
       </c>
       <c r="K30" t="inlineStr">
@@ -4129,7 +4129,7 @@
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>['Spain', 'Algeria', 'Brazil']</t>
+          <t>['Brazil', 'Spain', 'Algeria']</t>
         </is>
       </c>
       <c r="K31" t="inlineStr">
@@ -4257,7 +4257,7 @@
       </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t>['Spain', 'Northern Ireland', 'Brazil']</t>
+          <t>['Brazil', 'Spain', 'Northern Ireland']</t>
         </is>
       </c>
       <c r="K32" t="inlineStr">
@@ -4385,7 +4385,7 @@
       </c>
       <c r="J33" t="inlineStr">
         <is>
-          <t>['Spain', 'Algeria', 'Brazil']</t>
+          <t>['Brazil', 'Spain', 'Algeria']</t>
         </is>
       </c>
       <c r="K33" t="inlineStr">
@@ -4513,7 +4513,7 @@
       </c>
       <c r="J34" t="inlineStr">
         <is>
-          <t>['Spain', 'Northern Ireland', 'Brazil']</t>
+          <t>['Brazil', 'Spain', 'Northern Ireland']</t>
         </is>
       </c>
       <c r="K34" t="inlineStr">
@@ -4641,7 +4641,7 @@
       </c>
       <c r="J35" t="inlineStr">
         <is>
-          <t>['Spain', 'Northern Ireland', 'Brazil']</t>
+          <t>['Brazil', 'Spain', 'Northern Ireland']</t>
         </is>
       </c>
       <c r="K35" t="inlineStr">
@@ -4769,7 +4769,7 @@
       </c>
       <c r="J36" t="inlineStr">
         <is>
-          <t>['Spain', 'Northern Ireland', 'Brazil']</t>
+          <t>['Brazil', 'Spain', 'Northern Ireland']</t>
         </is>
       </c>
       <c r="K36" t="inlineStr">
@@ -4883,7 +4883,7 @@
       <c r="I37" t="inlineStr"/>
       <c r="J37" t="inlineStr">
         <is>
-          <t>['Uruguay', 'Denmark', 'West Germany']</t>
+          <t>['West Germany', 'Denmark', 'Uruguay']</t>
         </is>
       </c>
       <c r="K37" t="inlineStr">
@@ -4979,7 +4979,7 @@
       </c>
       <c r="J38" t="inlineStr">
         <is>
-          <t>['Uruguay', 'Denmark', 'West Germany']</t>
+          <t>['West Germany', 'Denmark', 'Uruguay']</t>
         </is>
       </c>
       <c r="K38" t="inlineStr">
@@ -5107,7 +5107,7 @@
       </c>
       <c r="J39" t="inlineStr">
         <is>
-          <t>['Uruguay', 'Denmark', 'West Germany']</t>
+          <t>['West Germany', 'Denmark', 'Uruguay']</t>
         </is>
       </c>
       <c r="K39" t="inlineStr">
@@ -5221,7 +5221,7 @@
       <c r="I40" t="inlineStr"/>
       <c r="J40" t="inlineStr">
         <is>
-          <t>['Argentina', 'Romania', 'Cameroon']</t>
+          <t>['Romania', 'Argentina', 'Cameroon']</t>
         </is>
       </c>
       <c r="K40" t="inlineStr">
@@ -5317,7 +5317,7 @@
       </c>
       <c r="J41" t="inlineStr">
         <is>
-          <t>['Argentina', 'Romania', 'Cameroon']</t>
+          <t>['Romania', 'Argentina', 'Cameroon']</t>
         </is>
       </c>
       <c r="K41" t="inlineStr">
@@ -5445,7 +5445,7 @@
       </c>
       <c r="J42" t="inlineStr">
         <is>
-          <t>['Argentina', 'Romania', 'Cameroon']</t>
+          <t>['Romania', 'Argentina', 'Cameroon']</t>
         </is>
       </c>
       <c r="K42" t="inlineStr">
@@ -5573,7 +5573,7 @@
       </c>
       <c r="J43" t="inlineStr">
         <is>
-          <t>['Argentina', 'Romania', 'Cameroon']</t>
+          <t>['Romania', 'Argentina', 'Cameroon']</t>
         </is>
       </c>
       <c r="K43" t="inlineStr">
@@ -5701,7 +5701,7 @@
       </c>
       <c r="J44" t="inlineStr">
         <is>
-          <t>['Cameroon', 'Romania', 'Argentina']</t>
+          <t>['Romania', 'Argentina', 'Cameroon']</t>
         </is>
       </c>
       <c r="K44" t="inlineStr">
@@ -5829,7 +5829,7 @@
       </c>
       <c r="J45" t="inlineStr">
         <is>
-          <t>['Cameroon', 'Soviet Union', 'Argentina']</t>
+          <t>['Argentina', 'Soviet Union', 'Cameroon']</t>
         </is>
       </c>
       <c r="K45" t="inlineStr">
@@ -5957,7 +5957,7 @@
       </c>
       <c r="J46" t="inlineStr">
         <is>
-          <t>['Argentina', 'Romania', 'Cameroon']</t>
+          <t>['Romania', 'Argentina', 'Cameroon']</t>
         </is>
       </c>
       <c r="K46" t="inlineStr">
@@ -6071,7 +6071,7 @@
       <c r="I47" t="inlineStr"/>
       <c r="J47" t="inlineStr">
         <is>
-          <t>['Colombia', 'Yugoslavia', 'West Germany']</t>
+          <t>['West Germany', 'Yugoslavia', 'Colombia']</t>
         </is>
       </c>
       <c r="K47" t="inlineStr">
@@ -6167,7 +6167,7 @@
       </c>
       <c r="J48" t="inlineStr">
         <is>
-          <t>['Colombia', 'Yugoslavia', 'West Germany']</t>
+          <t>['West Germany', 'Yugoslavia', 'Colombia']</t>
         </is>
       </c>
       <c r="K48" t="inlineStr">
@@ -6295,7 +6295,7 @@
       </c>
       <c r="J49" t="inlineStr">
         <is>
-          <t>['Colombia', 'Yugoslavia', 'West Germany']</t>
+          <t>['West Germany', 'Yugoslavia', 'Colombia']</t>
         </is>
       </c>
       <c r="K49" t="inlineStr">
@@ -6423,7 +6423,7 @@
       </c>
       <c r="J50" t="inlineStr">
         <is>
-          <t>['Colombia', 'Yugoslavia', 'West Germany']</t>
+          <t>['West Germany', 'Yugoslavia', 'Colombia']</t>
         </is>
       </c>
       <c r="K50" t="inlineStr">
@@ -6551,7 +6551,7 @@
       </c>
       <c r="J51" t="inlineStr">
         <is>
-          <t>['Colombia', 'Yugoslavia', 'West Germany']</t>
+          <t>['West Germany', 'Yugoslavia', 'Colombia']</t>
         </is>
       </c>
       <c r="K51" t="inlineStr">
@@ -6679,7 +6679,7 @@
       </c>
       <c r="J52" t="inlineStr">
         <is>
-          <t>['Colombia', 'Yugoslavia', 'West Germany']</t>
+          <t>['West Germany', 'Yugoslavia', 'Colombia']</t>
         </is>
       </c>
       <c r="K52" t="inlineStr">
@@ -6807,7 +6807,7 @@
       </c>
       <c r="J53" t="inlineStr">
         <is>
-          <t>['Colombia', 'Yugoslavia', 'West Germany']</t>
+          <t>['West Germany', 'Yugoslavia', 'Colombia']</t>
         </is>
       </c>
       <c r="K53" t="inlineStr">
@@ -6935,7 +6935,7 @@
       </c>
       <c r="J54" t="inlineStr">
         <is>
-          <t>['Colombia', 'Yugoslavia', 'West Germany']</t>
+          <t>['West Germany', 'Yugoslavia', 'Colombia']</t>
         </is>
       </c>
       <c r="K54" t="inlineStr">
@@ -7771,7 +7771,7 @@
       <c r="I61" t="inlineStr"/>
       <c r="J61" t="inlineStr">
         <is>
-          <t>['Costa Rica', 'Scotland', 'Brazil']</t>
+          <t>['Brazil', 'Scotland', 'Costa Rica']</t>
         </is>
       </c>
       <c r="K61" t="inlineStr">
@@ -7867,7 +7867,7 @@
       </c>
       <c r="J62" t="inlineStr">
         <is>
-          <t>['Sweden', 'Scotland', 'Brazil']</t>
+          <t>['Brazil', 'Sweden', 'Scotland']</t>
         </is>
       </c>
       <c r="K62" t="inlineStr">
@@ -7995,7 +7995,7 @@
       </c>
       <c r="J63" t="inlineStr">
         <is>
-          <t>['Scotland', 'Costa Rica', 'Brazil']</t>
+          <t>['Brazil', 'Scotland', 'Costa Rica']</t>
         </is>
       </c>
       <c r="K63" t="inlineStr">
@@ -8123,7 +8123,7 @@
       </c>
       <c r="J64" t="inlineStr">
         <is>
-          <t>['Scotland', 'Costa Rica', 'Brazil']</t>
+          <t>['Brazil', 'Scotland', 'Costa Rica']</t>
         </is>
       </c>
       <c r="K64" t="inlineStr">
@@ -8251,7 +8251,7 @@
       </c>
       <c r="J65" t="inlineStr">
         <is>
-          <t>['Scotland', 'Costa Rica', 'Brazil']</t>
+          <t>['Brazil', 'Scotland', 'Costa Rica']</t>
         </is>
       </c>
       <c r="K65" t="inlineStr">
@@ -8365,7 +8365,7 @@
       <c r="I66" t="inlineStr"/>
       <c r="J66" t="inlineStr">
         <is>
-          <t>['Belgium', 'Uruguay', 'Spain']</t>
+          <t>['Spain', 'Belgium', 'Uruguay']</t>
         </is>
       </c>
       <c r="K66" t="inlineStr">
@@ -8461,7 +8461,7 @@
       </c>
       <c r="J67" t="inlineStr">
         <is>
-          <t>['Belgium', 'Uruguay', 'Spain']</t>
+          <t>['Spain', 'Belgium', 'Uruguay']</t>
         </is>
       </c>
       <c r="K67" t="inlineStr">
@@ -8589,7 +8589,7 @@
       </c>
       <c r="J68" t="inlineStr">
         <is>
-          <t>['Belgium', 'Uruguay', 'Spain']</t>
+          <t>['Spain', 'Belgium', 'Uruguay']</t>
         </is>
       </c>
       <c r="K68" t="inlineStr">
@@ -8717,7 +8717,7 @@
       </c>
       <c r="J69" t="inlineStr">
         <is>
-          <t>['Belgium', 'Uruguay', 'Spain']</t>
+          <t>['Spain', 'Belgium', 'Uruguay']</t>
         </is>
       </c>
       <c r="K69" t="inlineStr">
@@ -8845,7 +8845,7 @@
       </c>
       <c r="J70" t="inlineStr">
         <is>
-          <t>['Belgium', 'Uruguay', 'Spain']</t>
+          <t>['Spain', 'Belgium', 'Uruguay']</t>
         </is>
       </c>
       <c r="K70" t="inlineStr">
@@ -8959,7 +8959,7 @@
       <c r="I71" t="inlineStr"/>
       <c r="J71" t="inlineStr">
         <is>
-          <t>['England', 'Netherlands', 'Ireland']</t>
+          <t>['Netherlands', 'Ireland', 'England']</t>
         </is>
       </c>
       <c r="K71" t="inlineStr">
@@ -9055,7 +9055,7 @@
       </c>
       <c r="J72" t="inlineStr">
         <is>
-          <t>['Egypt', 'England', 'Netherlands']</t>
+          <t>['Netherlands', 'Egypt', 'England']</t>
         </is>
       </c>
       <c r="K72" t="inlineStr">
@@ -9183,7 +9183,7 @@
       </c>
       <c r="J73" t="inlineStr">
         <is>
-          <t>['Egypt', 'England', 'Netherlands']</t>
+          <t>['Netherlands', 'Egypt', 'England']</t>
         </is>
       </c>
       <c r="K73" t="inlineStr">
@@ -9311,7 +9311,7 @@
       </c>
       <c r="J74" t="inlineStr">
         <is>
-          <t>['England', 'Netherlands', 'Ireland']</t>
+          <t>['Netherlands', 'Ireland', 'England']</t>
         </is>
       </c>
       <c r="K74" t="inlineStr">
@@ -9425,7 +9425,7 @@
       <c r="I75" t="inlineStr"/>
       <c r="J75" t="inlineStr">
         <is>
-          <t>['Switzerland', 'United States', 'Romania']</t>
+          <t>['Romania', 'United States', 'Switzerland']</t>
         </is>
       </c>
       <c r="K75" t="inlineStr">
@@ -9521,7 +9521,7 @@
       </c>
       <c r="J76" t="inlineStr">
         <is>
-          <t>['Switzerland', 'United States', 'Romania']</t>
+          <t>['United States', 'Romania', 'Switzerland']</t>
         </is>
       </c>
       <c r="K76" t="inlineStr">
@@ -9649,7 +9649,7 @@
       </c>
       <c r="J77" t="inlineStr">
         <is>
-          <t>['Switzerland', 'United States', 'Romania']</t>
+          <t>['United States', 'Romania', 'Switzerland']</t>
         </is>
       </c>
       <c r="K77" t="inlineStr">
@@ -9777,7 +9777,7 @@
       </c>
       <c r="J78" t="inlineStr">
         <is>
-          <t>['Switzerland', 'United States', 'Romania']</t>
+          <t>['United States', 'Romania', 'Switzerland']</t>
         </is>
       </c>
       <c r="K78" t="inlineStr">
@@ -9891,7 +9891,7 @@
       <c r="I79" t="inlineStr"/>
       <c r="J79" t="inlineStr">
         <is>
-          <t>['South Korea', 'Germany', 'Spain']</t>
+          <t>['South Korea', 'Spain', 'Germany']</t>
         </is>
       </c>
       <c r="K79" t="inlineStr">
@@ -9987,7 +9987,7 @@
       </c>
       <c r="J80" t="inlineStr">
         <is>
-          <t>['South Korea', 'Germany', 'Spain']</t>
+          <t>['South Korea', 'Spain', 'Germany']</t>
         </is>
       </c>
       <c r="K80" t="inlineStr">
@@ -10115,7 +10115,7 @@
       </c>
       <c r="J81" t="inlineStr">
         <is>
-          <t>['South Korea', 'Germany', 'Spain']</t>
+          <t>['South Korea', 'Spain', 'Germany']</t>
         </is>
       </c>
       <c r="K81" t="inlineStr">
@@ -10243,7 +10243,7 @@
       </c>
       <c r="J82" t="inlineStr">
         <is>
-          <t>['South Korea', 'Germany', 'Spain']</t>
+          <t>['South Korea', 'Spain', 'Germany']</t>
         </is>
       </c>
       <c r="K82" t="inlineStr">
@@ -10371,7 +10371,7 @@
       </c>
       <c r="J83" t="inlineStr">
         <is>
-          <t>['South Korea', 'Germany', 'Spain']</t>
+          <t>['South Korea', 'Spain', 'Germany']</t>
         </is>
       </c>
       <c r="K83" t="inlineStr">
@@ -10499,7 +10499,7 @@
       </c>
       <c r="J84" t="inlineStr">
         <is>
-          <t>['South Korea', 'Germany', 'Spain']</t>
+          <t>['South Korea', 'Spain', 'Germany']</t>
         </is>
       </c>
       <c r="K84" t="inlineStr">
@@ -10627,7 +10627,7 @@
       </c>
       <c r="J85" t="inlineStr">
         <is>
-          <t>['South Korea', 'Germany', 'Spain']</t>
+          <t>['South Korea', 'Spain', 'Germany']</t>
         </is>
       </c>
       <c r="K85" t="inlineStr">
@@ -10755,7 +10755,7 @@
       </c>
       <c r="J86" t="inlineStr">
         <is>
-          <t>['South Korea', 'Germany', 'Spain']</t>
+          <t>['South Korea', 'Spain', 'Germany']</t>
         </is>
       </c>
       <c r="K86" t="inlineStr">
@@ -10883,7 +10883,7 @@
       </c>
       <c r="J87" t="inlineStr">
         <is>
-          <t>['South Korea', 'Germany', 'Spain']</t>
+          <t>['South Korea', 'Spain', 'Germany']</t>
         </is>
       </c>
       <c r="K87" t="inlineStr">
@@ -11011,7 +11011,7 @@
       </c>
       <c r="J88" t="inlineStr">
         <is>
-          <t>['South Korea', 'Germany', 'Spain']</t>
+          <t>['South Korea', 'Spain', 'Germany']</t>
         </is>
       </c>
       <c r="K88" t="inlineStr">
@@ -11125,7 +11125,7 @@
       <c r="I89" t="inlineStr"/>
       <c r="J89" t="inlineStr">
         <is>
-          <t>['Mexico', 'Italy', 'Ireland']</t>
+          <t>['Italy', 'Ireland', 'Mexico']</t>
         </is>
       </c>
       <c r="K89" t="inlineStr">
@@ -11221,7 +11221,7 @@
       </c>
       <c r="J90" t="inlineStr">
         <is>
-          <t>['Norway', 'Italy', 'Ireland']</t>
+          <t>['Italy', 'Ireland', 'Norway']</t>
         </is>
       </c>
       <c r="K90" t="inlineStr">
@@ -11349,7 +11349,7 @@
       </c>
       <c r="J91" t="inlineStr">
         <is>
-          <t>['Mexico', 'Italy', 'Ireland']</t>
+          <t>['Italy', 'Ireland', 'Mexico']</t>
         </is>
       </c>
       <c r="K91" t="inlineStr">
@@ -11463,7 +11463,7 @@
       <c r="I92" t="inlineStr"/>
       <c r="J92" t="inlineStr">
         <is>
-          <t>['Sweden', 'Cameroon', 'Brazil']</t>
+          <t>['Brazil', 'Sweden', 'Cameroon']</t>
         </is>
       </c>
       <c r="K92" t="inlineStr">
@@ -11559,7 +11559,7 @@
       </c>
       <c r="J93" t="inlineStr">
         <is>
-          <t>['Sweden', 'Russia', 'Brazil']</t>
+          <t>['Brazil', 'Sweden', 'Russia']</t>
         </is>
       </c>
       <c r="K93" t="inlineStr">
@@ -11687,7 +11687,7 @@
       </c>
       <c r="J94" t="inlineStr">
         <is>
-          <t>['Sweden', 'Russia', 'Brazil']</t>
+          <t>['Sweden', 'Brazil', 'Russia']</t>
         </is>
       </c>
       <c r="K94" t="inlineStr">
@@ -11815,7 +11815,7 @@
       </c>
       <c r="J95" t="inlineStr">
         <is>
-          <t>['Sweden', 'Russia', 'Brazil']</t>
+          <t>['Sweden', 'Brazil', 'Russia']</t>
         </is>
       </c>
       <c r="K95" t="inlineStr">
@@ -11943,7 +11943,7 @@
       </c>
       <c r="J96" t="inlineStr">
         <is>
-          <t>['Sweden', 'Russia', 'Brazil']</t>
+          <t>['Sweden', 'Brazil', 'Russia']</t>
         </is>
       </c>
       <c r="K96" t="inlineStr">
@@ -12071,7 +12071,7 @@
       </c>
       <c r="J97" t="inlineStr">
         <is>
-          <t>['Sweden', 'Russia', 'Brazil']</t>
+          <t>['Sweden', 'Brazil', 'Russia']</t>
         </is>
       </c>
       <c r="K97" t="inlineStr">
@@ -12199,7 +12199,7 @@
       </c>
       <c r="J98" t="inlineStr">
         <is>
-          <t>['Sweden', 'Russia', 'Brazil']</t>
+          <t>['Brazil', 'Sweden', 'Russia']</t>
         </is>
       </c>
       <c r="K98" t="inlineStr">
@@ -12327,7 +12327,7 @@
       </c>
       <c r="J99" t="inlineStr">
         <is>
-          <t>['Sweden', 'Russia', 'Brazil']</t>
+          <t>['Brazil', 'Sweden', 'Russia']</t>
         </is>
       </c>
       <c r="K99" t="inlineStr">
@@ -12455,7 +12455,7 @@
       </c>
       <c r="J100" t="inlineStr">
         <is>
-          <t>['Sweden', 'Russia', 'Brazil']</t>
+          <t>['Brazil', 'Sweden', 'Russia']</t>
         </is>
       </c>
       <c r="K100" t="inlineStr">
@@ -12583,7 +12583,7 @@
       </c>
       <c r="J101" t="inlineStr">
         <is>
-          <t>['Sweden', 'Russia', 'Brazil']</t>
+          <t>['Brazil', 'Sweden', 'Russia']</t>
         </is>
       </c>
       <c r="K101" t="inlineStr">
@@ -12697,7 +12697,7 @@
       <c r="I102" t="inlineStr"/>
       <c r="J102" t="inlineStr">
         <is>
-          <t>['Belgium', 'Saudi Arabia', 'Netherlands']</t>
+          <t>['Netherlands', 'Saudi Arabia', 'Belgium']</t>
         </is>
       </c>
       <c r="K102" t="inlineStr">
@@ -12793,7 +12793,7 @@
       </c>
       <c r="J103" t="inlineStr">
         <is>
-          <t>['Saudi Arabia', 'Belgium', 'Netherlands']</t>
+          <t>['Netherlands', 'Saudi Arabia', 'Belgium']</t>
         </is>
       </c>
       <c r="K103" t="inlineStr">
@@ -12921,7 +12921,7 @@
       </c>
       <c r="J104" t="inlineStr">
         <is>
-          <t>['Saudi Arabia', 'Belgium', 'Netherlands']</t>
+          <t>['Netherlands', 'Saudi Arabia', 'Belgium']</t>
         </is>
       </c>
       <c r="K104" t="inlineStr">
@@ -13049,7 +13049,7 @@
       </c>
       <c r="J105" t="inlineStr">
         <is>
-          <t>['Saudi Arabia', 'Belgium', 'Netherlands']</t>
+          <t>['Netherlands', 'Saudi Arabia', 'Belgium']</t>
         </is>
       </c>
       <c r="K105" t="inlineStr">
@@ -13177,7 +13177,7 @@
       </c>
       <c r="J106" t="inlineStr">
         <is>
-          <t>['Saudi Arabia', 'Belgium', 'Netherlands']</t>
+          <t>['Netherlands', 'Saudi Arabia', 'Belgium']</t>
         </is>
       </c>
       <c r="K106" t="inlineStr">
@@ -13291,7 +13291,7 @@
       <c r="I107" t="inlineStr"/>
       <c r="J107" t="inlineStr">
         <is>
-          <t>['Bulgaria', 'Nigeria', 'Argentina']</t>
+          <t>['Nigeria', 'Argentina', 'Bulgaria']</t>
         </is>
       </c>
       <c r="K107" t="inlineStr">
@@ -13387,7 +13387,7 @@
       </c>
       <c r="J108" t="inlineStr">
         <is>
-          <t>['Bulgaria', 'Nigeria', 'Argentina']</t>
+          <t>['Nigeria', 'Argentina', 'Bulgaria']</t>
         </is>
       </c>
       <c r="K108" t="inlineStr">
@@ -13515,7 +13515,7 @@
       </c>
       <c r="J109" t="inlineStr">
         <is>
-          <t>['Bulgaria', 'Nigeria', 'Argentina']</t>
+          <t>['Nigeria', 'Argentina', 'Bulgaria']</t>
         </is>
       </c>
       <c r="K109" t="inlineStr">
@@ -13643,7 +13643,7 @@
       </c>
       <c r="J110" t="inlineStr">
         <is>
-          <t>['Bulgaria', 'Nigeria', 'Argentina']</t>
+          <t>['Nigeria', 'Argentina', 'Bulgaria']</t>
         </is>
       </c>
       <c r="K110" t="inlineStr">
@@ -13771,7 +13771,7 @@
       </c>
       <c r="J111" t="inlineStr">
         <is>
-          <t>['Bulgaria', 'Nigeria', 'Argentina']</t>
+          <t>['Nigeria', 'Argentina', 'Bulgaria']</t>
         </is>
       </c>
       <c r="K111" t="inlineStr">
@@ -13885,7 +13885,7 @@
       <c r="I112" t="inlineStr"/>
       <c r="J112" t="inlineStr">
         <is>
-          <t>['Chile', 'Italy']</t>
+          <t>['Italy', 'Chile']</t>
         </is>
       </c>
       <c r="K112" t="inlineStr">
@@ -13981,7 +13981,7 @@
       </c>
       <c r="J113" t="inlineStr">
         <is>
-          <t>['Chile', 'Italy']</t>
+          <t>['Italy', 'Chile']</t>
         </is>
       </c>
       <c r="K113" t="inlineStr">
@@ -14109,7 +14109,7 @@
       </c>
       <c r="J114" t="inlineStr">
         <is>
-          <t>['Chile', 'Italy']</t>
+          <t>['Italy', 'Chile']</t>
         </is>
       </c>
       <c r="K114" t="inlineStr">
@@ -14237,7 +14237,7 @@
       </c>
       <c r="J115" t="inlineStr">
         <is>
-          <t>['Chile', 'Italy']</t>
+          <t>['Italy', 'Chile']</t>
         </is>
       </c>
       <c r="K115" t="inlineStr">
@@ -14365,7 +14365,7 @@
       </c>
       <c r="J116" t="inlineStr">
         <is>
-          <t>['Chile', 'Italy']</t>
+          <t>['Italy', 'Chile']</t>
         </is>
       </c>
       <c r="K116" t="inlineStr">
@@ -14493,7 +14493,7 @@
       </c>
       <c r="J117" t="inlineStr">
         <is>
-          <t>['Chile', 'Italy']</t>
+          <t>['Italy', 'Chile']</t>
         </is>
       </c>
       <c r="K117" t="inlineStr">
@@ -14607,7 +14607,7 @@
       <c r="I118" t="inlineStr"/>
       <c r="J118" t="inlineStr">
         <is>
-          <t>['Norway', 'Brazil']</t>
+          <t>['Brazil', 'Norway']</t>
         </is>
       </c>
       <c r="K118" t="inlineStr">
@@ -15343,7 +15343,7 @@
       </c>
       <c r="J124" t="inlineStr">
         <is>
-          <t>['Norway', 'Brazil']</t>
+          <t>['Brazil', 'Norway']</t>
         </is>
       </c>
       <c r="K124" t="inlineStr">
@@ -16435,7 +16435,7 @@
       <c r="I133" t="inlineStr"/>
       <c r="J133" t="inlineStr">
         <is>
-          <t>['Paraguay', 'Nigeria']</t>
+          <t>['Nigeria', 'Paraguay']</t>
         </is>
       </c>
       <c r="K133" t="inlineStr">
@@ -16531,7 +16531,7 @@
       </c>
       <c r="J134" t="inlineStr">
         <is>
-          <t>['Paraguay', 'Nigeria']</t>
+          <t>['Nigeria', 'Paraguay']</t>
         </is>
       </c>
       <c r="K134" t="inlineStr">
@@ -16659,7 +16659,7 @@
       </c>
       <c r="J135" t="inlineStr">
         <is>
-          <t>['Paraguay', 'Nigeria']</t>
+          <t>['Nigeria', 'Paraguay']</t>
         </is>
       </c>
       <c r="K135" t="inlineStr">
@@ -17171,7 +17171,7 @@
       </c>
       <c r="J139" t="inlineStr">
         <is>
-          <t>['Paraguay', 'Nigeria']</t>
+          <t>['Nigeria', 'Paraguay']</t>
         </is>
       </c>
       <c r="K139" t="inlineStr">
@@ -17299,7 +17299,7 @@
       </c>
       <c r="J140" t="inlineStr">
         <is>
-          <t>['Paraguay', 'Nigeria']</t>
+          <t>['Nigeria', 'Paraguay']</t>
         </is>
       </c>
       <c r="K140" t="inlineStr">
@@ -17427,7 +17427,7 @@
       </c>
       <c r="J141" t="inlineStr">
         <is>
-          <t>['Paraguay', 'Nigeria']</t>
+          <t>['Nigeria', 'Paraguay']</t>
         </is>
       </c>
       <c r="K141" t="inlineStr">
@@ -17555,7 +17555,7 @@
       </c>
       <c r="J142" t="inlineStr">
         <is>
-          <t>['Paraguay', 'Nigeria']</t>
+          <t>['Nigeria', 'Paraguay']</t>
         </is>
       </c>
       <c r="K142" t="inlineStr">
@@ -17683,7 +17683,7 @@
       </c>
       <c r="J143" t="inlineStr">
         <is>
-          <t>['Paraguay', 'Nigeria']</t>
+          <t>['Nigeria', 'Paraguay']</t>
         </is>
       </c>
       <c r="K143" t="inlineStr">
@@ -17811,7 +17811,7 @@
       </c>
       <c r="J144" t="inlineStr">
         <is>
-          <t>['Paraguay', 'Nigeria']</t>
+          <t>['Nigeria', 'Paraguay']</t>
         </is>
       </c>
       <c r="K144" t="inlineStr">
@@ -17925,7 +17925,7 @@
       <c r="I145" t="inlineStr"/>
       <c r="J145" t="inlineStr">
         <is>
-          <t>['Mexico', 'Netherlands']</t>
+          <t>['Netherlands', 'Mexico']</t>
         </is>
       </c>
       <c r="K145" t="inlineStr">
@@ -18021,7 +18021,7 @@
       </c>
       <c r="J146" t="inlineStr">
         <is>
-          <t>['Mexico', 'Netherlands']</t>
+          <t>['Netherlands', 'Mexico']</t>
         </is>
       </c>
       <c r="K146" t="inlineStr">
@@ -18149,7 +18149,7 @@
       </c>
       <c r="J147" t="inlineStr">
         <is>
-          <t>['Belgium', 'Netherlands']</t>
+          <t>['Netherlands', 'Belgium']</t>
         </is>
       </c>
       <c r="K147" t="inlineStr">
@@ -18277,7 +18277,7 @@
       </c>
       <c r="J148" t="inlineStr">
         <is>
-          <t>['Belgium', 'Netherlands']</t>
+          <t>['Netherlands', 'Belgium']</t>
         </is>
       </c>
       <c r="K148" t="inlineStr">
@@ -18405,7 +18405,7 @@
       </c>
       <c r="J149" t="inlineStr">
         <is>
-          <t>['Mexico', 'Netherlands']</t>
+          <t>['Netherlands', 'Mexico']</t>
         </is>
       </c>
       <c r="K149" t="inlineStr">
@@ -18533,7 +18533,7 @@
       </c>
       <c r="J150" t="inlineStr">
         <is>
-          <t>['Mexico', 'Netherlands']</t>
+          <t>['Netherlands', 'Mexico']</t>
         </is>
       </c>
       <c r="K150" t="inlineStr">
@@ -18661,7 +18661,7 @@
       </c>
       <c r="J151" t="inlineStr">
         <is>
-          <t>['Mexico', 'Netherlands']</t>
+          <t>['Netherlands', 'Mexico']</t>
         </is>
       </c>
       <c r="K151" t="inlineStr">
@@ -19241,7 +19241,7 @@
       <c r="I156" t="inlineStr"/>
       <c r="J156" t="inlineStr">
         <is>
-          <t>['Croatia', 'Argentina']</t>
+          <t>['Argentina', 'Croatia']</t>
         </is>
       </c>
       <c r="K156" t="inlineStr">
@@ -19337,7 +19337,7 @@
       </c>
       <c r="J157" t="inlineStr">
         <is>
-          <t>['Croatia', 'Argentina']</t>
+          <t>['Argentina', 'Croatia']</t>
         </is>
       </c>
       <c r="K157" t="inlineStr">
@@ -19465,7 +19465,7 @@
       </c>
       <c r="J158" t="inlineStr">
         <is>
-          <t>['Croatia', 'Argentina']</t>
+          <t>['Argentina', 'Croatia']</t>
         </is>
       </c>
       <c r="K158" t="inlineStr">
@@ -19593,7 +19593,7 @@
       </c>
       <c r="J159" t="inlineStr">
         <is>
-          <t>['Croatia', 'Argentina']</t>
+          <t>['Argentina', 'Croatia']</t>
         </is>
       </c>
       <c r="K159" t="inlineStr">
@@ -19721,7 +19721,7 @@
       </c>
       <c r="J160" t="inlineStr">
         <is>
-          <t>['Croatia', 'Argentina']</t>
+          <t>['Argentina', 'Croatia']</t>
         </is>
       </c>
       <c r="K160" t="inlineStr">
@@ -19835,7 +19835,7 @@
       <c r="I161" t="inlineStr"/>
       <c r="J161" t="inlineStr">
         <is>
-          <t>['England', 'Romania']</t>
+          <t>['Romania', 'England']</t>
         </is>
       </c>
       <c r="K161" t="inlineStr">
@@ -19931,7 +19931,7 @@
       </c>
       <c r="J162" t="inlineStr">
         <is>
-          <t>['England', 'Romania']</t>
+          <t>['Romania', 'England']</t>
         </is>
       </c>
       <c r="K162" t="inlineStr">
@@ -20059,7 +20059,7 @@
       </c>
       <c r="J163" t="inlineStr">
         <is>
-          <t>['England', 'Romania']</t>
+          <t>['Romania', 'England']</t>
         </is>
       </c>
       <c r="K163" t="inlineStr">
@@ -20187,7 +20187,7 @@
       </c>
       <c r="J164" t="inlineStr">
         <is>
-          <t>['England', 'Romania']</t>
+          <t>['Romania', 'England']</t>
         </is>
       </c>
       <c r="K164" t="inlineStr">
@@ -20315,7 +20315,7 @@
       </c>
       <c r="J165" t="inlineStr">
         <is>
-          <t>['England', 'Romania']</t>
+          <t>['Romania', 'England']</t>
         </is>
       </c>
       <c r="K165" t="inlineStr">
@@ -21631,7 +21631,7 @@
       </c>
       <c r="J176" t="inlineStr">
         <is>
-          <t>['Germany', 'Ireland']</t>
+          <t>['Ireland', 'Germany']</t>
         </is>
       </c>
       <c r="K176" t="inlineStr">
@@ -21759,7 +21759,7 @@
       </c>
       <c r="J177" t="inlineStr">
         <is>
-          <t>['Germany', 'Ireland']</t>
+          <t>['Ireland', 'Germany']</t>
         </is>
       </c>
       <c r="K177" t="inlineStr">
@@ -21887,7 +21887,7 @@
       </c>
       <c r="J178" t="inlineStr">
         <is>
-          <t>['Germany', 'Ireland']</t>
+          <t>['Ireland', 'Germany']</t>
         </is>
       </c>
       <c r="K178" t="inlineStr">
@@ -22015,7 +22015,7 @@
       </c>
       <c r="J179" t="inlineStr">
         <is>
-          <t>['Germany', 'Ireland']</t>
+          <t>['Ireland', 'Germany']</t>
         </is>
       </c>
       <c r="K179" t="inlineStr">
@@ -22143,7 +22143,7 @@
       </c>
       <c r="J180" t="inlineStr">
         <is>
-          <t>['Germany', 'Ireland']</t>
+          <t>['Ireland', 'Germany']</t>
         </is>
       </c>
       <c r="K180" t="inlineStr">
@@ -23829,7 +23829,7 @@
       <c r="I194" t="inlineStr"/>
       <c r="J194" t="inlineStr">
         <is>
-          <t>['Costa Rica', 'Brazil']</t>
+          <t>['Brazil', 'Costa Rica']</t>
         </is>
       </c>
       <c r="K194" t="inlineStr">
@@ -23925,7 +23925,7 @@
       </c>
       <c r="J195" t="inlineStr">
         <is>
-          <t>['Costa Rica', 'Brazil']</t>
+          <t>['Brazil', 'Costa Rica']</t>
         </is>
       </c>
       <c r="K195" t="inlineStr">
@@ -24053,7 +24053,7 @@
       </c>
       <c r="J196" t="inlineStr">
         <is>
-          <t>['Costa Rica', 'Brazil']</t>
+          <t>['Brazil', 'Costa Rica']</t>
         </is>
       </c>
       <c r="K196" t="inlineStr">
@@ -24181,7 +24181,7 @@
       </c>
       <c r="J197" t="inlineStr">
         <is>
-          <t>['Turkey', 'Brazil']</t>
+          <t>['Brazil', 'Turkey']</t>
         </is>
       </c>
       <c r="K197" t="inlineStr">
@@ -24309,7 +24309,7 @@
       </c>
       <c r="J198" t="inlineStr">
         <is>
-          <t>['Turkey', 'Brazil']</t>
+          <t>['Brazil', 'Turkey']</t>
         </is>
       </c>
       <c r="K198" t="inlineStr">
@@ -24437,7 +24437,7 @@
       </c>
       <c r="J199" t="inlineStr">
         <is>
-          <t>['Turkey', 'Brazil']</t>
+          <t>['Brazil', 'Turkey']</t>
         </is>
       </c>
       <c r="K199" t="inlineStr">
@@ -24565,7 +24565,7 @@
       </c>
       <c r="J200" t="inlineStr">
         <is>
-          <t>['Turkey', 'Brazil']</t>
+          <t>['Brazil', 'Turkey']</t>
         </is>
       </c>
       <c r="K200" t="inlineStr">
@@ -24693,7 +24693,7 @@
       </c>
       <c r="J201" t="inlineStr">
         <is>
-          <t>['Costa Rica', 'Brazil']</t>
+          <t>['Brazil', 'Costa Rica']</t>
         </is>
       </c>
       <c r="K201" t="inlineStr">
@@ -24821,7 +24821,7 @@
       </c>
       <c r="J202" t="inlineStr">
         <is>
-          <t>['Turkey', 'Brazil']</t>
+          <t>['Brazil', 'Turkey']</t>
         </is>
       </c>
       <c r="K202" t="inlineStr">
@@ -24949,7 +24949,7 @@
       </c>
       <c r="J203" t="inlineStr">
         <is>
-          <t>['Turkey', 'Brazil']</t>
+          <t>['Brazil', 'Turkey']</t>
         </is>
       </c>
       <c r="K203" t="inlineStr">
@@ -25077,7 +25077,7 @@
       </c>
       <c r="J204" t="inlineStr">
         <is>
-          <t>['Turkey', 'Brazil']</t>
+          <t>['Brazil', 'Turkey']</t>
         </is>
       </c>
       <c r="K204" t="inlineStr">
@@ -25191,7 +25191,7 @@
       <c r="I205" t="inlineStr"/>
       <c r="J205" t="inlineStr">
         <is>
-          <t>['Mexico', 'Italy']</t>
+          <t>['Italy', 'Mexico']</t>
         </is>
       </c>
       <c r="K205" t="inlineStr">
@@ -25415,7 +25415,7 @@
       </c>
       <c r="J207" t="inlineStr">
         <is>
-          <t>['Mexico', 'Italy']</t>
+          <t>['Italy', 'Mexico']</t>
         </is>
       </c>
       <c r="K207" t="inlineStr">
@@ -25543,7 +25543,7 @@
       </c>
       <c r="J208" t="inlineStr">
         <is>
-          <t>['Mexico', 'Italy']</t>
+          <t>['Italy', 'Mexico']</t>
         </is>
       </c>
       <c r="K208" t="inlineStr">
@@ -25881,7 +25881,7 @@
       </c>
       <c r="J211" t="inlineStr">
         <is>
-          <t>['Japan', 'Belgium']</t>
+          <t>['Belgium', 'Japan']</t>
         </is>
       </c>
       <c r="K211" t="inlineStr">
@@ -26265,7 +26265,7 @@
       </c>
       <c r="J214" t="inlineStr">
         <is>
-          <t>['Japan', 'Belgium']</t>
+          <t>['Belgium', 'Japan']</t>
         </is>
       </c>
       <c r="K214" t="inlineStr">
@@ -26393,7 +26393,7 @@
       </c>
       <c r="J215" t="inlineStr">
         <is>
-          <t>['Japan', 'Belgium']</t>
+          <t>['Belgium', 'Japan']</t>
         </is>
       </c>
       <c r="K215" t="inlineStr">
@@ -26521,7 +26521,7 @@
       </c>
       <c r="J216" t="inlineStr">
         <is>
-          <t>['Japan', 'Belgium']</t>
+          <t>['Belgium', 'Japan']</t>
         </is>
       </c>
       <c r="K216" t="inlineStr">
@@ -26635,7 +26635,7 @@
       <c r="I217" t="inlineStr"/>
       <c r="J217" t="inlineStr">
         <is>
-          <t>['South Korea', 'United States']</t>
+          <t>['United States', 'South Korea']</t>
         </is>
       </c>
       <c r="K217" t="inlineStr">
@@ -26731,7 +26731,7 @@
       </c>
       <c r="J218" t="inlineStr">
         <is>
-          <t>['South Korea', 'Portugal']</t>
+          <t>['Portugal', 'South Korea']</t>
         </is>
       </c>
       <c r="K218" t="inlineStr">
@@ -26859,7 +26859,7 @@
       </c>
       <c r="J219" t="inlineStr">
         <is>
-          <t>['South Korea', 'Portugal']</t>
+          <t>['Portugal', 'South Korea']</t>
         </is>
       </c>
       <c r="K219" t="inlineStr">
@@ -26987,7 +26987,7 @@
       </c>
       <c r="J220" t="inlineStr">
         <is>
-          <t>['South Korea', 'Portugal']</t>
+          <t>['Portugal', 'South Korea']</t>
         </is>
       </c>
       <c r="K220" t="inlineStr">
@@ -27115,7 +27115,7 @@
       </c>
       <c r="J221" t="inlineStr">
         <is>
-          <t>['South Korea', 'United States']</t>
+          <t>['United States', 'South Korea']</t>
         </is>
       </c>
       <c r="K221" t="inlineStr">
@@ -27243,7 +27243,7 @@
       </c>
       <c r="J222" t="inlineStr">
         <is>
-          <t>['South Korea', 'United States']</t>
+          <t>['United States', 'South Korea']</t>
         </is>
       </c>
       <c r="K222" t="inlineStr">
@@ -30501,7 +30501,7 @@
       <c r="I249" t="inlineStr"/>
       <c r="J249" t="inlineStr">
         <is>
-          <t>['Italy', 'Czech Republic']</t>
+          <t>['Czech Republic', 'Italy']</t>
         </is>
       </c>
       <c r="K249" t="inlineStr">
@@ -30597,7 +30597,7 @@
       </c>
       <c r="J250" t="inlineStr">
         <is>
-          <t>['Ghana', 'Italy']</t>
+          <t>['Italy', 'Ghana']</t>
         </is>
       </c>
       <c r="K250" t="inlineStr">
@@ -30725,7 +30725,7 @@
       </c>
       <c r="J251" t="inlineStr">
         <is>
-          <t>['Ghana', 'Italy']</t>
+          <t>['Italy', 'Ghana']</t>
         </is>
       </c>
       <c r="K251" t="inlineStr">
@@ -30853,7 +30853,7 @@
       </c>
       <c r="J252" t="inlineStr">
         <is>
-          <t>['Ghana', 'Italy']</t>
+          <t>['Italy', 'Ghana']</t>
         </is>
       </c>
       <c r="K252" t="inlineStr">
@@ -30981,7 +30981,7 @@
       </c>
       <c r="J253" t="inlineStr">
         <is>
-          <t>['Ghana', 'Italy']</t>
+          <t>['Italy', 'Ghana']</t>
         </is>
       </c>
       <c r="K253" t="inlineStr">
@@ -31109,7 +31109,7 @@
       </c>
       <c r="J254" t="inlineStr">
         <is>
-          <t>['Ghana', 'Italy']</t>
+          <t>['Italy', 'Ghana']</t>
         </is>
       </c>
       <c r="K254" t="inlineStr">
@@ -31223,7 +31223,7 @@
       <c r="I255" t="inlineStr"/>
       <c r="J255" t="inlineStr">
         <is>
-          <t>['Australia', 'Brazil']</t>
+          <t>['Brazil', 'Australia']</t>
         </is>
       </c>
       <c r="K255" t="inlineStr">
@@ -31319,7 +31319,7 @@
       </c>
       <c r="J256" t="inlineStr">
         <is>
-          <t>['Croatia', 'Brazil']</t>
+          <t>['Brazil', 'Croatia']</t>
         </is>
       </c>
       <c r="K256" t="inlineStr">
@@ -31447,7 +31447,7 @@
       </c>
       <c r="J257" t="inlineStr">
         <is>
-          <t>['Croatia', 'Brazil']</t>
+          <t>['Brazil', 'Croatia']</t>
         </is>
       </c>
       <c r="K257" t="inlineStr">
@@ -31575,7 +31575,7 @@
       </c>
       <c r="J258" t="inlineStr">
         <is>
-          <t>['Australia', 'Brazil']</t>
+          <t>['Brazil', 'Australia']</t>
         </is>
       </c>
       <c r="K258" t="inlineStr">
@@ -31703,7 +31703,7 @@
       </c>
       <c r="J259" t="inlineStr">
         <is>
-          <t>['Australia', 'Brazil']</t>
+          <t>['Brazil', 'Australia']</t>
         </is>
       </c>
       <c r="K259" t="inlineStr">
@@ -31831,7 +31831,7 @@
       </c>
       <c r="J260" t="inlineStr">
         <is>
-          <t>['Australia', 'Brazil']</t>
+          <t>['Brazil', 'Australia']</t>
         </is>
       </c>
       <c r="K260" t="inlineStr">
@@ -31959,7 +31959,7 @@
       </c>
       <c r="J261" t="inlineStr">
         <is>
-          <t>['Croatia', 'Brazil']</t>
+          <t>['Brazil', 'Croatia']</t>
         </is>
       </c>
       <c r="K261" t="inlineStr">
@@ -32087,7 +32087,7 @@
       </c>
       <c r="J262" t="inlineStr">
         <is>
-          <t>['Croatia', 'Brazil']</t>
+          <t>['Brazil', 'Croatia']</t>
         </is>
       </c>
       <c r="K262" t="inlineStr">
@@ -32215,7 +32215,7 @@
       </c>
       <c r="J263" t="inlineStr">
         <is>
-          <t>['Australia', 'Brazil']</t>
+          <t>['Brazil', 'Australia']</t>
         </is>
       </c>
       <c r="K263" t="inlineStr">
@@ -32343,7 +32343,7 @@
       </c>
       <c r="J264" t="inlineStr">
         <is>
-          <t>['Australia', 'Brazil']</t>
+          <t>['Brazil', 'Australia']</t>
         </is>
       </c>
       <c r="K264" t="inlineStr">
@@ -32795,7 +32795,7 @@
       <c r="I268" t="inlineStr"/>
       <c r="J268" t="inlineStr">
         <is>
-          <t>['South Korea', 'Switzerland']</t>
+          <t>['Switzerland', 'South Korea']</t>
         </is>
       </c>
       <c r="K268" t="inlineStr">
@@ -32891,7 +32891,7 @@
       </c>
       <c r="J269" t="inlineStr">
         <is>
-          <t>['South Korea', 'Switzerland']</t>
+          <t>['Switzerland', 'South Korea']</t>
         </is>
       </c>
       <c r="K269" t="inlineStr">
@@ -33983,7 +33983,7 @@
       <c r="I278" t="inlineStr"/>
       <c r="J278" t="inlineStr">
         <is>
-          <t>['South Korea', 'Argentina']</t>
+          <t>['Argentina', 'South Korea']</t>
         </is>
       </c>
       <c r="K278" t="inlineStr">
@@ -34079,7 +34079,7 @@
       </c>
       <c r="J279" t="inlineStr">
         <is>
-          <t>['Greece', 'Argentina']</t>
+          <t>['Argentina', 'Greece']</t>
         </is>
       </c>
       <c r="K279" t="inlineStr">
@@ -34207,7 +34207,7 @@
       </c>
       <c r="J280" t="inlineStr">
         <is>
-          <t>['South Korea', 'Argentina']</t>
+          <t>['Argentina', 'South Korea']</t>
         </is>
       </c>
       <c r="K280" t="inlineStr">
@@ -34335,7 +34335,7 @@
       </c>
       <c r="J281" t="inlineStr">
         <is>
-          <t>['South Korea', 'Argentina']</t>
+          <t>['Argentina', 'South Korea']</t>
         </is>
       </c>
       <c r="K281" t="inlineStr">
@@ -34463,7 +34463,7 @@
       </c>
       <c r="J282" t="inlineStr">
         <is>
-          <t>['South Korea', 'Argentina']</t>
+          <t>['Argentina', 'South Korea']</t>
         </is>
       </c>
       <c r="K282" t="inlineStr">
@@ -34591,7 +34591,7 @@
       </c>
       <c r="J283" t="inlineStr">
         <is>
-          <t>['South Korea', 'Argentina']</t>
+          <t>['Argentina', 'South Korea']</t>
         </is>
       </c>
       <c r="K283" t="inlineStr">
@@ -34719,7 +34719,7 @@
       </c>
       <c r="J284" t="inlineStr">
         <is>
-          <t>['South Korea', 'Argentina']</t>
+          <t>['Argentina', 'South Korea']</t>
         </is>
       </c>
       <c r="K284" t="inlineStr">
@@ -34929,7 +34929,7 @@
       </c>
       <c r="J286" t="inlineStr">
         <is>
-          <t>['England', 'Slovenia']</t>
+          <t>['Slovenia', 'England']</t>
         </is>
       </c>
       <c r="K286" t="inlineStr">
@@ -35057,7 +35057,7 @@
       </c>
       <c r="J287" t="inlineStr">
         <is>
-          <t>['England', 'United States']</t>
+          <t>['United States', 'England']</t>
         </is>
       </c>
       <c r="K287" t="inlineStr">
@@ -35171,7 +35171,7 @@
       <c r="I288" t="inlineStr"/>
       <c r="J288" t="inlineStr">
         <is>
-          <t>['Ghana', 'Germany']</t>
+          <t>['Germany', 'Ghana']</t>
         </is>
       </c>
       <c r="K288" t="inlineStr">
@@ -35267,7 +35267,7 @@
       </c>
       <c r="J289" t="inlineStr">
         <is>
-          <t>['Ghana', 'Germany']</t>
+          <t>['Germany', 'Ghana']</t>
         </is>
       </c>
       <c r="K289" t="inlineStr">
@@ -35395,7 +35395,7 @@
       </c>
       <c r="J290" t="inlineStr">
         <is>
-          <t>['Ghana', 'Germany']</t>
+          <t>['Germany', 'Ghana']</t>
         </is>
       </c>
       <c r="K290" t="inlineStr">
@@ -35523,7 +35523,7 @@
       </c>
       <c r="J291" t="inlineStr">
         <is>
-          <t>['Ghana', 'Germany']</t>
+          <t>['Germany', 'Ghana']</t>
         </is>
       </c>
       <c r="K291" t="inlineStr">
@@ -35651,7 +35651,7 @@
       </c>
       <c r="J292" t="inlineStr">
         <is>
-          <t>['Ghana', 'Germany']</t>
+          <t>['Germany', 'Ghana']</t>
         </is>
       </c>
       <c r="K292" t="inlineStr">
@@ -35765,7 +35765,7 @@
       <c r="I293" t="inlineStr"/>
       <c r="J293" t="inlineStr">
         <is>
-          <t>['Paraguay', 'Italy']</t>
+          <t>['Italy', 'Paraguay']</t>
         </is>
       </c>
       <c r="K293" t="inlineStr">
@@ -36487,7 +36487,7 @@
       <c r="I299" t="inlineStr"/>
       <c r="J299" t="inlineStr">
         <is>
-          <t>['Japan', 'Netherlands']</t>
+          <t>['Netherlands', 'Japan']</t>
         </is>
       </c>
       <c r="K299" t="inlineStr">
@@ -36583,7 +36583,7 @@
       </c>
       <c r="J300" t="inlineStr">
         <is>
-          <t>['Japan', 'Netherlands']</t>
+          <t>['Netherlands', 'Japan']</t>
         </is>
       </c>
       <c r="K300" t="inlineStr">
@@ -36711,7 +36711,7 @@
       </c>
       <c r="J301" t="inlineStr">
         <is>
-          <t>['Japan', 'Netherlands']</t>
+          <t>['Netherlands', 'Japan']</t>
         </is>
       </c>
       <c r="K301" t="inlineStr">
@@ -36839,7 +36839,7 @@
       </c>
       <c r="J302" t="inlineStr">
         <is>
-          <t>['Japan', 'Netherlands']</t>
+          <t>['Netherlands', 'Japan']</t>
         </is>
       </c>
       <c r="K302" t="inlineStr">
@@ -36967,7 +36967,7 @@
       </c>
       <c r="J303" t="inlineStr">
         <is>
-          <t>['Japan', 'Netherlands']</t>
+          <t>['Netherlands', 'Japan']</t>
         </is>
       </c>
       <c r="K303" t="inlineStr">
@@ -37095,7 +37095,7 @@
       </c>
       <c r="J304" t="inlineStr">
         <is>
-          <t>['Japan', 'Netherlands']</t>
+          <t>['Netherlands', 'Japan']</t>
         </is>
       </c>
       <c r="K304" t="inlineStr">
@@ -37223,7 +37223,7 @@
       </c>
       <c r="J305" t="inlineStr">
         <is>
-          <t>['Japan', 'Netherlands']</t>
+          <t>['Netherlands', 'Japan']</t>
         </is>
       </c>
       <c r="K305" t="inlineStr">
@@ -37351,7 +37351,7 @@
       </c>
       <c r="J306" t="inlineStr">
         <is>
-          <t>['Japan', 'Netherlands']</t>
+          <t>['Netherlands', 'Japan']</t>
         </is>
       </c>
       <c r="K306" t="inlineStr">
@@ -37465,7 +37465,7 @@
       <c r="I307" t="inlineStr"/>
       <c r="J307" t="inlineStr">
         <is>
-          <t>['Portugal', 'Brazil']</t>
+          <t>['Brazil', 'Portugal']</t>
         </is>
       </c>
       <c r="K307" t="inlineStr">
@@ -37561,7 +37561,7 @@
       </c>
       <c r="J308" t="inlineStr">
         <is>
-          <t>['Portugal', 'Brazil']</t>
+          <t>['Brazil', 'Portugal']</t>
         </is>
       </c>
       <c r="K308" t="inlineStr">
@@ -37689,7 +37689,7 @@
       </c>
       <c r="J309" t="inlineStr">
         <is>
-          <t>['Portugal', 'Brazil']</t>
+          <t>['Brazil', 'Portugal']</t>
         </is>
       </c>
       <c r="K309" t="inlineStr">
@@ -37817,7 +37817,7 @@
       </c>
       <c r="J310" t="inlineStr">
         <is>
-          <t>['Portugal', 'Brazil']</t>
+          <t>['Brazil', 'Portugal']</t>
         </is>
       </c>
       <c r="K310" t="inlineStr">
@@ -38397,7 +38397,7 @@
       <c r="I315" t="inlineStr"/>
       <c r="J315" t="inlineStr">
         <is>
-          <t>['Chile', 'Netherlands']</t>
+          <t>['Netherlands', 'Chile']</t>
         </is>
       </c>
       <c r="K315" t="inlineStr">
@@ -38493,7 +38493,7 @@
       </c>
       <c r="J316" t="inlineStr">
         <is>
-          <t>['Chile', 'Netherlands']</t>
+          <t>['Netherlands', 'Chile']</t>
         </is>
       </c>
       <c r="K316" t="inlineStr">
@@ -38621,7 +38621,7 @@
       </c>
       <c r="J317" t="inlineStr">
         <is>
-          <t>['Chile', 'Netherlands']</t>
+          <t>['Netherlands', 'Chile']</t>
         </is>
       </c>
       <c r="K317" t="inlineStr">
@@ -38749,7 +38749,7 @@
       </c>
       <c r="J318" t="inlineStr">
         <is>
-          <t>['Chile', 'Netherlands']</t>
+          <t>['Netherlands', 'Chile']</t>
         </is>
       </c>
       <c r="K318" t="inlineStr">
@@ -38877,7 +38877,7 @@
       </c>
       <c r="J319" t="inlineStr">
         <is>
-          <t>['Chile', 'Netherlands']</t>
+          <t>['Netherlands', 'Chile']</t>
         </is>
       </c>
       <c r="K319" t="inlineStr">
@@ -39005,7 +39005,7 @@
       </c>
       <c r="J320" t="inlineStr">
         <is>
-          <t>['Chile', 'Netherlands']</t>
+          <t>['Netherlands', 'Chile']</t>
         </is>
       </c>
       <c r="K320" t="inlineStr">
@@ -39119,7 +39119,7 @@
       <c r="I321" t="inlineStr"/>
       <c r="J321" t="inlineStr">
         <is>
-          <t>['Mexico', 'Brazil']</t>
+          <t>['Brazil', 'Mexico']</t>
         </is>
       </c>
       <c r="K321" t="inlineStr">
@@ -39215,7 +39215,7 @@
       </c>
       <c r="J322" t="inlineStr">
         <is>
-          <t>['Mexico', 'Brazil']</t>
+          <t>['Brazil', 'Mexico']</t>
         </is>
       </c>
       <c r="K322" t="inlineStr">
@@ -39343,7 +39343,7 @@
       </c>
       <c r="J323" t="inlineStr">
         <is>
-          <t>['Mexico', 'Brazil']</t>
+          <t>['Brazil', 'Mexico']</t>
         </is>
       </c>
       <c r="K323" t="inlineStr">
@@ -39471,7 +39471,7 @@
       </c>
       <c r="J324" t="inlineStr">
         <is>
-          <t>['Mexico', 'Brazil']</t>
+          <t>['Brazil', 'Mexico']</t>
         </is>
       </c>
       <c r="K324" t="inlineStr">
@@ -39599,7 +39599,7 @@
       </c>
       <c r="J325" t="inlineStr">
         <is>
-          <t>['Mexico', 'Brazil']</t>
+          <t>['Brazil', 'Mexico']</t>
         </is>
       </c>
       <c r="K325" t="inlineStr">
@@ -39727,7 +39727,7 @@
       </c>
       <c r="J326" t="inlineStr">
         <is>
-          <t>['Mexico', 'Brazil']</t>
+          <t>['Brazil', 'Mexico']</t>
         </is>
       </c>
       <c r="K326" t="inlineStr">
@@ -39855,7 +39855,7 @@
       </c>
       <c r="J327" t="inlineStr">
         <is>
-          <t>['Mexico', 'Brazil']</t>
+          <t>['Brazil', 'Mexico']</t>
         </is>
       </c>
       <c r="K327" t="inlineStr">
@@ -39983,7 +39983,7 @@
       </c>
       <c r="J328" t="inlineStr">
         <is>
-          <t>['Mexico', 'Brazil']</t>
+          <t>['Brazil', 'Mexico']</t>
         </is>
       </c>
       <c r="K328" t="inlineStr">
@@ -40111,7 +40111,7 @@
       </c>
       <c r="J329" t="inlineStr">
         <is>
-          <t>['Mexico', 'Brazil']</t>
+          <t>['Brazil', 'Mexico']</t>
         </is>
       </c>
       <c r="K329" t="inlineStr">
@@ -40239,7 +40239,7 @@
       </c>
       <c r="J330" t="inlineStr">
         <is>
-          <t>['Mexico', 'Brazil']</t>
+          <t>['Brazil', 'Mexico']</t>
         </is>
       </c>
       <c r="K330" t="inlineStr">
@@ -40449,7 +40449,7 @@
       </c>
       <c r="J332" t="inlineStr">
         <is>
-          <t>['Uruguay', 'Costa Rica']</t>
+          <t>['Costa Rica', 'Uruguay']</t>
         </is>
       </c>
       <c r="K332" t="inlineStr">
@@ -40563,7 +40563,7 @@
       <c r="I333" t="inlineStr"/>
       <c r="J333" t="inlineStr">
         <is>
-          <t>['Colombia', 'Ivory Coast']</t>
+          <t>['Ivory Coast', 'Colombia']</t>
         </is>
       </c>
       <c r="K333" t="inlineStr">
@@ -40659,7 +40659,7 @@
       </c>
       <c r="J334" t="inlineStr">
         <is>
-          <t>['Colombia', 'Ivory Coast']</t>
+          <t>['Ivory Coast', 'Colombia']</t>
         </is>
       </c>
       <c r="K334" t="inlineStr">
@@ -40787,7 +40787,7 @@
       </c>
       <c r="J335" t="inlineStr">
         <is>
-          <t>['Greece', 'Colombia']</t>
+          <t>['Colombia', 'Greece']</t>
         </is>
       </c>
       <c r="K335" t="inlineStr">
@@ -40915,7 +40915,7 @@
       </c>
       <c r="J336" t="inlineStr">
         <is>
-          <t>['Greece', 'Colombia']</t>
+          <t>['Colombia', 'Greece']</t>
         </is>
       </c>
       <c r="K336" t="inlineStr">
@@ -41043,7 +41043,7 @@
       </c>
       <c r="J337" t="inlineStr">
         <is>
-          <t>['Greece', 'Colombia']</t>
+          <t>['Colombia', 'Greece']</t>
         </is>
       </c>
       <c r="K337" t="inlineStr">
@@ -41171,7 +41171,7 @@
       </c>
       <c r="J338" t="inlineStr">
         <is>
-          <t>['Colombia', 'Ivory Coast']</t>
+          <t>['Ivory Coast', 'Colombia']</t>
         </is>
       </c>
       <c r="K338" t="inlineStr">
@@ -41299,7 +41299,7 @@
       </c>
       <c r="J339" t="inlineStr">
         <is>
-          <t>['Colombia', 'Ivory Coast']</t>
+          <t>['Ivory Coast', 'Colombia']</t>
         </is>
       </c>
       <c r="K339" t="inlineStr">
@@ -41427,7 +41427,7 @@
       </c>
       <c r="J340" t="inlineStr">
         <is>
-          <t>['Colombia', 'Ivory Coast']</t>
+          <t>['Ivory Coast', 'Colombia']</t>
         </is>
       </c>
       <c r="K340" t="inlineStr">
@@ -41555,7 +41555,7 @@
       </c>
       <c r="J341" t="inlineStr">
         <is>
-          <t>['Greece', 'Colombia']</t>
+          <t>['Colombia', 'Greece']</t>
         </is>
       </c>
       <c r="K341" t="inlineStr">
@@ -43369,7 +43369,7 @@
       <c r="I356" t="inlineStr"/>
       <c r="J356" t="inlineStr">
         <is>
-          <t>['Germany', 'United States']</t>
+          <t>['United States', 'Germany']</t>
         </is>
       </c>
       <c r="K356" t="inlineStr">
@@ -43465,7 +43465,7 @@
       </c>
       <c r="J357" t="inlineStr">
         <is>
-          <t>['Germany', 'United States']</t>
+          <t>['United States', 'Germany']</t>
         </is>
       </c>
       <c r="K357" t="inlineStr">
@@ -43593,7 +43593,7 @@
       </c>
       <c r="J358" t="inlineStr">
         <is>
-          <t>['Germany', 'United States']</t>
+          <t>['United States', 'Germany']</t>
         </is>
       </c>
       <c r="K358" t="inlineStr">
@@ -43721,7 +43721,7 @@
       </c>
       <c r="J359" t="inlineStr">
         <is>
-          <t>['Germany', 'United States']</t>
+          <t>['United States', 'Germany']</t>
         </is>
       </c>
       <c r="K359" t="inlineStr">
@@ -43849,7 +43849,7 @@
       </c>
       <c r="J360" t="inlineStr">
         <is>
-          <t>['Germany', 'United States']</t>
+          <t>['United States', 'Germany']</t>
         </is>
       </c>
       <c r="K360" t="inlineStr">
@@ -44059,7 +44059,7 @@
       </c>
       <c r="J362" t="inlineStr">
         <is>
-          <t>['Russia', 'Belgium']</t>
+          <t>['Belgium', 'Russia']</t>
         </is>
       </c>
       <c r="K362" t="inlineStr">
@@ -44429,7 +44429,7 @@
       <c r="I365" t="inlineStr"/>
       <c r="J365" t="inlineStr">
         <is>
-          <t>['Russia', 'Uruguay']</t>
+          <t>['Uruguay', 'Russia']</t>
         </is>
       </c>
       <c r="K365" t="inlineStr">
@@ -46563,7 +46563,7 @@
       </c>
       <c r="J383" t="inlineStr">
         <is>
-          <t>['Croatia', 'Argentina']</t>
+          <t>['Argentina', 'Croatia']</t>
         </is>
       </c>
       <c r="K383" t="inlineStr">
@@ -47075,7 +47075,7 @@
       </c>
       <c r="J387" t="inlineStr">
         <is>
-          <t>['Croatia', 'Argentina']</t>
+          <t>['Argentina', 'Croatia']</t>
         </is>
       </c>
       <c r="K387" t="inlineStr">
@@ -47203,7 +47203,7 @@
       </c>
       <c r="J388" t="inlineStr">
         <is>
-          <t>['Croatia', 'Argentina']</t>
+          <t>['Argentina', 'Croatia']</t>
         </is>
       </c>
       <c r="K388" t="inlineStr">
@@ -47317,7 +47317,7 @@
       <c r="I389" t="inlineStr"/>
       <c r="J389" t="inlineStr">
         <is>
-          <t>['Germany', 'Mexico']</t>
+          <t>['Mexico', 'Germany']</t>
         </is>
       </c>
       <c r="K389" t="inlineStr">
@@ -48039,7 +48039,7 @@
       <c r="I395" t="inlineStr"/>
       <c r="J395" t="inlineStr">
         <is>
-          <t>['Switzerland', 'Brazil']</t>
+          <t>['Brazil', 'Switzerland']</t>
         </is>
       </c>
       <c r="K395" t="inlineStr">
@@ -48135,7 +48135,7 @@
       </c>
       <c r="J396" t="inlineStr">
         <is>
-          <t>['Switzerland', 'Brazil']</t>
+          <t>['Brazil', 'Switzerland']</t>
         </is>
       </c>
       <c r="K396" t="inlineStr">
@@ -48263,7 +48263,7 @@
       </c>
       <c r="J397" t="inlineStr">
         <is>
-          <t>['Switzerland', 'Brazil']</t>
+          <t>['Brazil', 'Switzerland']</t>
         </is>
       </c>
       <c r="K397" t="inlineStr">
@@ -48391,7 +48391,7 @@
       </c>
       <c r="J398" t="inlineStr">
         <is>
-          <t>['Switzerland', 'Brazil']</t>
+          <t>['Brazil', 'Switzerland']</t>
         </is>
       </c>
       <c r="K398" t="inlineStr">
@@ -48519,7 +48519,7 @@
       </c>
       <c r="J399" t="inlineStr">
         <is>
-          <t>['Switzerland', 'Brazil']</t>
+          <t>['Brazil', 'Switzerland']</t>
         </is>
       </c>
       <c r="K399" t="inlineStr">
@@ -48647,7 +48647,7 @@
       </c>
       <c r="J400" t="inlineStr">
         <is>
-          <t>['Switzerland', 'Brazil']</t>
+          <t>['Brazil', 'Switzerland']</t>
         </is>
       </c>
       <c r="K400" t="inlineStr">
@@ -48775,7 +48775,7 @@
       </c>
       <c r="J401" t="inlineStr">
         <is>
-          <t>['Switzerland', 'Brazil']</t>
+          <t>['Brazil', 'Switzerland']</t>
         </is>
       </c>
       <c r="K401" t="inlineStr">
@@ -48889,7 +48889,7 @@
       <c r="I402" t="inlineStr"/>
       <c r="J402" t="inlineStr">
         <is>
-          <t>['Japan', 'Senegal']</t>
+          <t>['Senegal', 'Japan']</t>
         </is>
       </c>
       <c r="K402" t="inlineStr">
@@ -48985,7 +48985,7 @@
       </c>
       <c r="J403" t="inlineStr">
         <is>
-          <t>['Colombia', 'Senegal']</t>
+          <t>['Senegal', 'Colombia']</t>
         </is>
       </c>
       <c r="K403" t="inlineStr">
@@ -49113,7 +49113,7 @@
       </c>
       <c r="J404" t="inlineStr">
         <is>
-          <t>['Colombia', 'Senegal']</t>
+          <t>['Senegal', 'Colombia']</t>
         </is>
       </c>
       <c r="K404" t="inlineStr">
@@ -49821,7 +49821,7 @@
       <c r="I410" t="inlineStr"/>
       <c r="J410" t="inlineStr">
         <is>
-          <t>['Ecuador', 'Netherlands']</t>
+          <t>['Netherlands', 'Ecuador']</t>
         </is>
       </c>
       <c r="K410" t="inlineStr">
@@ -49917,7 +49917,7 @@
       </c>
       <c r="J411" t="inlineStr">
         <is>
-          <t>['Ecuador', 'Netherlands']</t>
+          <t>['Netherlands', 'Ecuador']</t>
         </is>
       </c>
       <c r="K411" t="inlineStr">
@@ -50045,7 +50045,7 @@
       </c>
       <c r="J412" t="inlineStr">
         <is>
-          <t>['Senegal', 'Netherlands']</t>
+          <t>['Netherlands', 'Senegal']</t>
         </is>
       </c>
       <c r="K412" t="inlineStr">
@@ -50173,7 +50173,7 @@
       </c>
       <c r="J413" t="inlineStr">
         <is>
-          <t>['Senegal', 'Netherlands']</t>
+          <t>['Netherlands', 'Senegal']</t>
         </is>
       </c>
       <c r="K413" t="inlineStr">
@@ -50301,7 +50301,7 @@
       </c>
       <c r="J414" t="inlineStr">
         <is>
-          <t>['Ecuador', 'Netherlands']</t>
+          <t>['Netherlands', 'Ecuador']</t>
         </is>
       </c>
       <c r="K414" t="inlineStr">
@@ -50429,7 +50429,7 @@
       </c>
       <c r="J415" t="inlineStr">
         <is>
-          <t>['Senegal', 'Netherlands']</t>
+          <t>['Netherlands', 'Senegal']</t>
         </is>
       </c>
       <c r="K415" t="inlineStr">
@@ -50543,7 +50543,7 @@
       <c r="I416" t="inlineStr"/>
       <c r="J416" t="inlineStr">
         <is>
-          <t>['England', 'Iran']</t>
+          <t>['Iran', 'England']</t>
         </is>
       </c>
       <c r="K416" t="inlineStr">
@@ -50639,7 +50639,7 @@
       </c>
       <c r="J417" t="inlineStr">
         <is>
-          <t>['England', 'United States']</t>
+          <t>['United States', 'England']</t>
         </is>
       </c>
       <c r="K417" t="inlineStr">
@@ -50767,7 +50767,7 @@
       </c>
       <c r="J418" t="inlineStr">
         <is>
-          <t>['England', 'United States']</t>
+          <t>['United States', 'England']</t>
         </is>
       </c>
       <c r="K418" t="inlineStr">
@@ -50895,7 +50895,7 @@
       </c>
       <c r="J419" t="inlineStr">
         <is>
-          <t>['England', 'United States']</t>
+          <t>['United States', 'England']</t>
         </is>
       </c>
       <c r="K419" t="inlineStr">
@@ -51023,7 +51023,7 @@
       </c>
       <c r="J420" t="inlineStr">
         <is>
-          <t>['England', 'United States']</t>
+          <t>['United States', 'England']</t>
         </is>
       </c>
       <c r="K420" t="inlineStr">
@@ -51137,7 +51137,7 @@
       <c r="I421" t="inlineStr"/>
       <c r="J421" t="inlineStr">
         <is>
-          <t>['Australia', 'France']</t>
+          <t>['France', 'Australia']</t>
         </is>
       </c>
       <c r="K421" t="inlineStr">
@@ -51233,7 +51233,7 @@
       </c>
       <c r="J422" t="inlineStr">
         <is>
-          <t>['Tunisia', 'France']</t>
+          <t>['France', 'Tunisia']</t>
         </is>
       </c>
       <c r="K422" t="inlineStr">
@@ -51361,7 +51361,7 @@
       </c>
       <c r="J423" t="inlineStr">
         <is>
-          <t>['Australia', 'France']</t>
+          <t>['France', 'Australia']</t>
         </is>
       </c>
       <c r="K423" t="inlineStr">
@@ -52197,7 +52197,7 @@
       <c r="I430" t="inlineStr"/>
       <c r="J430" t="inlineStr">
         <is>
-          <t>['Croatia', 'Morocco']</t>
+          <t>['Morocco', 'Croatia']</t>
         </is>
       </c>
       <c r="K430" t="inlineStr">
@@ -52293,7 +52293,7 @@
       </c>
       <c r="J431" t="inlineStr">
         <is>
-          <t>['Croatia', 'Morocco']</t>
+          <t>['Morocco', 'Croatia']</t>
         </is>
       </c>
       <c r="K431" t="inlineStr">
@@ -52421,7 +52421,7 @@
       </c>
       <c r="J432" t="inlineStr">
         <is>
-          <t>['Croatia', 'Morocco']</t>
+          <t>['Morocco', 'Croatia']</t>
         </is>
       </c>
       <c r="K432" t="inlineStr">
@@ -52549,7 +52549,7 @@
       </c>
       <c r="J433" t="inlineStr">
         <is>
-          <t>['Croatia', 'Morocco']</t>
+          <t>['Morocco', 'Croatia']</t>
         </is>
       </c>
       <c r="K433" t="inlineStr">
@@ -52663,7 +52663,7 @@
       <c r="I434" t="inlineStr"/>
       <c r="J434" t="inlineStr">
         <is>
-          <t>['Japan', 'Spain']</t>
+          <t>['Spain', 'Japan']</t>
         </is>
       </c>
       <c r="K434" t="inlineStr">
@@ -52759,7 +52759,7 @@
       </c>
       <c r="J435" t="inlineStr">
         <is>
-          <t>['Germany', 'Spain']</t>
+          <t>['Spain', 'Germany']</t>
         </is>
       </c>
       <c r="K435" t="inlineStr">
@@ -52887,7 +52887,7 @@
       </c>
       <c r="J436" t="inlineStr">
         <is>
-          <t>['Germany', 'Spain']</t>
+          <t>['Spain', 'Germany']</t>
         </is>
       </c>
       <c r="K436" t="inlineStr">
@@ -53015,7 +53015,7 @@
       </c>
       <c r="J437" t="inlineStr">
         <is>
-          <t>['Japan', 'Spain']</t>
+          <t>['Spain', 'Japan']</t>
         </is>
       </c>
       <c r="K437" t="inlineStr">
@@ -53143,7 +53143,7 @@
       </c>
       <c r="J438" t="inlineStr">
         <is>
-          <t>['Japan', 'Spain']</t>
+          <t>['Spain', 'Japan']</t>
         </is>
       </c>
       <c r="K438" t="inlineStr">
@@ -53271,7 +53271,7 @@
       </c>
       <c r="J439" t="inlineStr">
         <is>
-          <t>['Japan', 'Spain']</t>
+          <t>['Spain', 'Japan']</t>
         </is>
       </c>
       <c r="K439" t="inlineStr">
@@ -53399,7 +53399,7 @@
       </c>
       <c r="J440" t="inlineStr">
         <is>
-          <t>['Japan', 'Costa Rica']</t>
+          <t>['Costa Rica', 'Japan']</t>
         </is>
       </c>
       <c r="K440" t="inlineStr">
@@ -53527,7 +53527,7 @@
       </c>
       <c r="J441" t="inlineStr">
         <is>
-          <t>['Japan', 'Spain']</t>
+          <t>['Spain', 'Japan']</t>
         </is>
       </c>
       <c r="K441" t="inlineStr">
@@ -53655,7 +53655,7 @@
       </c>
       <c r="J442" t="inlineStr">
         <is>
-          <t>['Japan', 'Spain']</t>
+          <t>['Spain', 'Japan']</t>
         </is>
       </c>
       <c r="K442" t="inlineStr">
@@ -53783,7 +53783,7 @@
       </c>
       <c r="J443" t="inlineStr">
         <is>
-          <t>['Japan', 'Spain']</t>
+          <t>['Spain', 'Japan']</t>
         </is>
       </c>
       <c r="K443" t="inlineStr">
@@ -53897,7 +53897,7 @@
       <c r="I444" t="inlineStr"/>
       <c r="J444" t="inlineStr">
         <is>
-          <t>['Ghana', 'Portugal']</t>
+          <t>['Portugal', 'Ghana']</t>
         </is>
       </c>
       <c r="K444" t="inlineStr">
@@ -53993,7 +53993,7 @@
       </c>
       <c r="J445" t="inlineStr">
         <is>
-          <t>['Ghana', 'Portugal']</t>
+          <t>['Portugal', 'Ghana']</t>
         </is>
       </c>
       <c r="K445" t="inlineStr">
@@ -54505,7 +54505,7 @@
       </c>
       <c r="J449" t="inlineStr">
         <is>
-          <t>['South Korea', 'Portugal']</t>
+          <t>['Portugal', 'South Korea']</t>
         </is>
       </c>
       <c r="K449" t="inlineStr">
@@ -54619,7 +54619,7 @@
       <c r="I450" t="inlineStr"/>
       <c r="J450" t="inlineStr">
         <is>
-          <t>['Switzerland', 'Brazil']</t>
+          <t>['Brazil', 'Switzerland']</t>
         </is>
       </c>
       <c r="K450" t="inlineStr">
@@ -54715,7 +54715,7 @@
       </c>
       <c r="J451" t="inlineStr">
         <is>
-          <t>['Switzerland', 'Brazil']</t>
+          <t>['Brazil', 'Switzerland']</t>
         </is>
       </c>
       <c r="K451" t="inlineStr">
@@ -54843,7 +54843,7 @@
       </c>
       <c r="J452" t="inlineStr">
         <is>
-          <t>['Switzerland', 'Brazil']</t>
+          <t>['Brazil', 'Switzerland']</t>
         </is>
       </c>
       <c r="K452" t="inlineStr">
@@ -54971,7 +54971,7 @@
       </c>
       <c r="J453" t="inlineStr">
         <is>
-          <t>['Serbia', 'Brazil']</t>
+          <t>['Brazil', 'Serbia']</t>
         </is>
       </c>
       <c r="K453" t="inlineStr">
@@ -55099,7 +55099,7 @@
       </c>
       <c r="J454" t="inlineStr">
         <is>
-          <t>['Switzerland', 'Brazil']</t>
+          <t>['Brazil', 'Switzerland']</t>
         </is>
       </c>
       <c r="K454" t="inlineStr">
@@ -55227,7 +55227,7 @@
       </c>
       <c r="J455" t="inlineStr">
         <is>
-          <t>['Switzerland', 'Brazil']</t>
+          <t>['Brazil', 'Switzerland']</t>
         </is>
       </c>
       <c r="K455" t="inlineStr">
@@ -55355,7 +55355,7 @@
       </c>
       <c r="J456" t="inlineStr">
         <is>
-          <t>['Switzerland', 'Brazil']</t>
+          <t>['Brazil', 'Switzerland']</t>
         </is>
       </c>
       <c r="K456" t="inlineStr">

</xml_diff>